<commit_message>
Final version: Admin password bimal@123 + Student view only + Push from doels server
</commit_message>
<xml_diff>
--- a/BTS306.CA.xlsx
+++ b/BTS306.CA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\CA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3EBFA8-0A57-4A37-8B4F-543E9D36A4DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF9F1D8-A1DB-486D-B7AD-F311CFEADBC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -599,21 +599,6 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>11</v>
-      </c>
-      <c r="F2">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>7</v>
-      </c>
-      <c r="H2">
-        <v>9</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -625,21 +610,6 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
-      <c r="G3">
-        <v>6</v>
-      </c>
-      <c r="H3">
-        <v>9</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -651,21 +621,6 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -677,21 +632,6 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>14</v>
-      </c>
-      <c r="F5">
-        <v>6</v>
-      </c>
-      <c r="G5">
-        <v>9</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -703,21 +643,6 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>9</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>7</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -729,21 +654,6 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>14</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>7</v>
-      </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -755,21 +665,6 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>8</v>
-      </c>
-      <c r="F8">
-        <v>8</v>
-      </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>8</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -781,21 +676,6 @@
       <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <v>9</v>
-      </c>
-      <c r="F9">
-        <v>6</v>
-      </c>
-      <c r="G9">
-        <v>9</v>
-      </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -807,21 +687,6 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="D10">
-        <v>12</v>
-      </c>
-      <c r="E10">
-        <v>13</v>
-      </c>
-      <c r="F10">
-        <v>6</v>
-      </c>
-      <c r="G10">
-        <v>10</v>
-      </c>
-      <c r="H10">
-        <v>8</v>
-      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -833,21 +698,6 @@
       <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11">
-        <v>6</v>
-      </c>
-      <c r="G11">
-        <v>7</v>
-      </c>
-      <c r="H11">
-        <v>9</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -859,21 +709,6 @@
       <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D12">
-        <v>8</v>
-      </c>
-      <c r="E12">
-        <v>8</v>
-      </c>
-      <c r="F12">
-        <v>7</v>
-      </c>
-      <c r="G12">
-        <v>8</v>
-      </c>
-      <c r="H12">
-        <v>10</v>
-      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -885,21 +720,6 @@
       <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="D13">
-        <v>11</v>
-      </c>
-      <c r="E13">
-        <v>13</v>
-      </c>
-      <c r="F13">
-        <v>10</v>
-      </c>
-      <c r="G13">
-        <v>6</v>
-      </c>
-      <c r="H13">
-        <v>6</v>
-      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -911,21 +731,6 @@
       <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D14">
-        <v>8</v>
-      </c>
-      <c r="E14">
-        <v>12</v>
-      </c>
-      <c r="F14">
-        <v>8</v>
-      </c>
-      <c r="G14">
-        <v>9</v>
-      </c>
-      <c r="H14">
-        <v>10</v>
-      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -937,21 +742,6 @@
       <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="D15">
-        <v>11</v>
-      </c>
-      <c r="E15">
-        <v>13</v>
-      </c>
-      <c r="F15">
-        <v>7</v>
-      </c>
-      <c r="G15">
-        <v>6</v>
-      </c>
-      <c r="H15">
-        <v>6</v>
-      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
@@ -963,23 +753,8 @@
       <c r="C16" t="s">
         <v>10</v>
       </c>
-      <c r="D16">
-        <v>14</v>
-      </c>
-      <c r="E16">
-        <v>15</v>
-      </c>
-      <c r="F16">
-        <v>9</v>
-      </c>
-      <c r="G16">
-        <v>10</v>
-      </c>
-      <c r="H16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -989,23 +764,8 @@
       <c r="C17" t="s">
         <v>10</v>
       </c>
-      <c r="D17">
-        <v>10</v>
-      </c>
-      <c r="E17">
-        <v>14</v>
-      </c>
-      <c r="F17">
-        <v>6</v>
-      </c>
-      <c r="G17">
-        <v>8</v>
-      </c>
-      <c r="H17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
@@ -1015,23 +775,8 @@
       <c r="C18" t="s">
         <v>10</v>
       </c>
-      <c r="D18">
-        <v>11</v>
-      </c>
-      <c r="E18">
-        <v>9</v>
-      </c>
-      <c r="F18">
-        <v>8</v>
-      </c>
-      <c r="G18">
-        <v>5</v>
-      </c>
-      <c r="H18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -1041,23 +786,8 @@
       <c r="C19" t="s">
         <v>10</v>
       </c>
-      <c r="D19">
-        <v>13</v>
-      </c>
-      <c r="E19">
-        <v>11</v>
-      </c>
-      <c r="F19">
-        <v>9</v>
-      </c>
-      <c r="G19">
-        <v>8</v>
-      </c>
-      <c r="H19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -1067,23 +797,8 @@
       <c r="C20" t="s">
         <v>10</v>
       </c>
-      <c r="D20">
-        <v>9</v>
-      </c>
-      <c r="E20">
-        <v>9</v>
-      </c>
-      <c r="F20">
-        <v>6</v>
-      </c>
-      <c r="G20">
-        <v>8</v>
-      </c>
-      <c r="H20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
@@ -1093,23 +808,8 @@
       <c r="C21" t="s">
         <v>13</v>
       </c>
-      <c r="D21">
-        <v>13</v>
-      </c>
-      <c r="E21">
-        <v>10</v>
-      </c>
-      <c r="F21">
-        <v>8</v>
-      </c>
-      <c r="G21">
-        <v>8</v>
-      </c>
-      <c r="H21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1119,23 +819,8 @@
       <c r="C22" t="s">
         <v>13</v>
       </c>
-      <c r="D22">
-        <v>8</v>
-      </c>
-      <c r="E22">
-        <v>11</v>
-      </c>
-      <c r="F22">
-        <v>5</v>
-      </c>
-      <c r="G22">
-        <v>8</v>
-      </c>
-      <c r="H22">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
@@ -1145,23 +830,8 @@
       <c r="C23" t="s">
         <v>13</v>
       </c>
-      <c r="D23">
-        <v>10</v>
-      </c>
-      <c r="E23">
-        <v>13</v>
-      </c>
-      <c r="F23">
-        <v>10</v>
-      </c>
-      <c r="G23">
-        <v>10</v>
-      </c>
-      <c r="H23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -1171,23 +841,8 @@
       <c r="C24" t="s">
         <v>10</v>
       </c>
-      <c r="D24">
-        <v>10</v>
-      </c>
-      <c r="E24">
-        <v>8</v>
-      </c>
-      <c r="F24">
-        <v>9</v>
-      </c>
-      <c r="G24">
-        <v>10</v>
-      </c>
-      <c r="H24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>56</v>
       </c>
@@ -1197,23 +852,8 @@
       <c r="C25" t="s">
         <v>13</v>
       </c>
-      <c r="D25">
-        <v>9</v>
-      </c>
-      <c r="E25">
-        <v>12</v>
-      </c>
-      <c r="F25">
-        <v>8</v>
-      </c>
-      <c r="G25">
-        <v>10</v>
-      </c>
-      <c r="H25">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
@@ -1223,23 +863,8 @@
       <c r="C26" t="s">
         <v>13</v>
       </c>
-      <c r="D26">
-        <v>11</v>
-      </c>
-      <c r="E26">
-        <v>8</v>
-      </c>
-      <c r="F26">
-        <v>7</v>
-      </c>
-      <c r="G26">
-        <v>10</v>
-      </c>
-      <c r="H26">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
@@ -1248,21 +873,6 @@
       </c>
       <c r="C27" t="s">
         <v>10</v>
-      </c>
-      <c r="D27">
-        <v>13</v>
-      </c>
-      <c r="E27">
-        <v>8</v>
-      </c>
-      <c r="F27">
-        <v>10</v>
-      </c>
-      <c r="G27">
-        <v>8</v>
-      </c>
-      <c r="H27">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>